<commit_message>
add model selection and boosting
</commit_message>
<xml_diff>
--- a/Data_science_project_checklist.xlsx
+++ b/Data_science_project_checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\st\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\st\Desktop\2018_docs\ML\ML-A-Z\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD8BE73-DC59-472B-BABE-1DAB0554D4D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4F0BE1-05D7-4DB9-A4E2-CA06D2138020}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10180" xr2:uid="{97177BAF-258B-4A32-9A4B-20C6F28510F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{97177BAF-258B-4A32-9A4B-20C6F28510F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Activity</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Compare models developed so far and analyze the failure cases</t>
   </si>
   <si>
-    <t>### Model validation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Generate independent validation sets (entirely different from training data) for testing </t>
   </si>
   <si>
@@ -103,6 +100,18 @@
   </si>
   <si>
     <t>Apply feature selection methods - PCA , LDA etc</t>
+  </si>
+  <si>
+    <t>Model selection</t>
+  </si>
+  <si>
+    <t>### Model validation(K-fold validation,.etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">### Model imprvement using grid search </t>
+  </si>
+  <si>
+    <t>### Model boosting using XGBoost or other techniques</t>
   </si>
 </sst>
 </file>
@@ -154,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -192,19 +201,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -234,6 +230,34 @@
       </right>
       <top/>
       <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -242,19 +266,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,28 +594,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49B41B00-4349-450A-9B8E-09BA0A0B1B59}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="89.81640625" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5"/>
@@ -633,7 +658,7 @@
       <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5"/>
@@ -658,7 +683,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5"/>
     </row>
@@ -693,38 +718,54 @@
       <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
       <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="9" t="s">
-        <v>17</v>
+      <c r="A21" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="6"/>
-    </row>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="11"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>